<commit_message>
Excel sheet updated with Android auto commands
</commit_message>
<xml_diff>
--- a/textDataset.xlsx
+++ b/textDataset.xlsx
@@ -20,15 +20,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">find a Hotel near me</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select destination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">find a ATM Near me</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">Play my 'Driving at night' playlist"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Play country music"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Play Frank Sinatra"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Play Planet Money on NPR One."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Play Adele Radio on iHeartRadio."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Navigate to Union Square, San Francisco."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Directions to Philz Coffee."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Drive to 1600 Amphitheatre Parkway, Mountain View."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Message Cody White on Hangouts."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Message Cody White on Whatsapp."</t>
   </si>
 </sst>
 </file>
@@ -38,7 +59,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -59,11 +80,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,7 +129,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -134,16 +150,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.7295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.1938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.1938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -159,6 +176,41 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>